<commit_message>
All Info of 14 Stores Updated
</commit_message>
<xml_diff>
--- a/Calling_Trees/Calling Tree - Aug-25.xlsx
+++ b/Calling_Trees/Calling Tree - Aug-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://xclusivetrading-my.sharepoint.com/personal/m_mahee_xclusivetradinginc_com/Documents/Desktop/Python/Calling Tree Dashboard/CallingTree_Dashboard/Calling_Trees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{443089ED-E8E2-44A4-B672-0F8AB15D6A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{056B5E21-CCFF-43BE-9265-32509609DB68}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{443089ED-E8E2-44A4-B672-0F8AB15D6A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F5BD554-2DE5-4B46-9E06-F14E64EEA9FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4229" uniqueCount="1556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4307" uniqueCount="1585">
   <si>
     <t>S.NO</t>
   </si>
@@ -4707,6 +4707,93 @@
   </si>
   <si>
     <t>4063 HIALEAH</t>
+  </si>
+  <si>
+    <t>Rinaldi@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>Desoto@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>11865sw@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>14317dixie@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>17225NW@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>1834NE@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>2014NE@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>2410federal@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>3056southstate@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>310Washington@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>501palm@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>6705taft@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>7258SW@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>8765sw@xclusivetradinginc.com</t>
+  </si>
+  <si>
+    <t>Takover in Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (818) 471-4211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (818) 480-5042</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9517</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9196</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9027</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9041</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9109</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (954) 645-7099</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (754) 218-0189</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9056</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9067</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (954) 545-7162</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9751</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +1 (786) 652-9740</t>
   </si>
 </sst>
 </file>
@@ -5284,37 +5371,37 @@
   </sheetPr>
   <dimension ref="A1:X253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="68" style="6" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="68" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="44" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -8687,9 +8774,15 @@
       <c r="J46" s="4" t="s">
         <v>1515</v>
       </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="K46" s="4">
+        <v>10211200</v>
+      </c>
+      <c r="L46" s="4">
+        <v>70856248</v>
+      </c>
+      <c r="M46" s="4">
+        <v>6870780</v>
+      </c>
       <c r="N46" s="4" t="s">
         <v>1005</v>
       </c>
@@ -8702,15 +8795,27 @@
       <c r="Q46" s="4" t="s">
         <v>1511</v>
       </c>
-      <c r="R46" s="4"/>
+      <c r="R46" s="4">
+        <v>82038750</v>
+      </c>
       <c r="S46" s="4" t="s">
         <v>1516</v>
       </c>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4"/>
-      <c r="W46" s="5"/>
-      <c r="X46" s="8"/>
+      <c r="T46" s="4">
+        <v>688</v>
+      </c>
+      <c r="U46" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>1556</v>
+      </c>
+      <c r="W46" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X46" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="47" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
@@ -8744,9 +8849,15 @@
       <c r="J47" s="4" t="s">
         <v>1514</v>
       </c>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="K47" s="4">
+        <v>10231989</v>
+      </c>
+      <c r="L47" s="4">
+        <v>70856249</v>
+      </c>
+      <c r="M47" s="4">
+        <v>7347295</v>
+      </c>
       <c r="N47" s="4" t="s">
         <v>1005</v>
       </c>
@@ -8759,15 +8870,27 @@
       <c r="Q47" s="4" t="s">
         <v>1511</v>
       </c>
-      <c r="R47" s="4"/>
+      <c r="R47" s="4">
+        <v>82038751</v>
+      </c>
       <c r="S47" s="4" t="s">
         <v>1517</v>
       </c>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="8"/>
+      <c r="T47" s="4">
+        <v>689</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="W47" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X47" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="48" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
@@ -20282,15 +20405,22 @@
       </c>
     </row>
     <row r="204" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="4"/>
+      <c r="A204" s="4">
+        <f t="shared" si="4"/>
+        <v>203</v>
+      </c>
       <c r="B204" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D204" s="4"/>
-      <c r="E204" s="4"/>
+      <c r="D204" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F204" s="4" t="s">
         <v>28</v>
       </c>
@@ -20306,9 +20436,15 @@
       <c r="J204" s="4" t="s">
         <v>1542</v>
       </c>
-      <c r="K204" s="4"/>
-      <c r="L204" s="4"/>
-      <c r="M204" s="4"/>
+      <c r="K204" s="4">
+        <v>10210174</v>
+      </c>
+      <c r="L204" s="4">
+        <v>70856261</v>
+      </c>
+      <c r="M204" s="4">
+        <v>1826134</v>
+      </c>
       <c r="N204" s="4" t="s">
         <v>762</v>
       </c>
@@ -20318,27 +20454,48 @@
       <c r="P204" s="4" t="s">
         <v>1518</v>
       </c>
-      <c r="Q204" s="4"/>
-      <c r="R204" s="4"/>
+      <c r="Q204" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R204" s="4">
+        <v>82038763</v>
+      </c>
       <c r="S204" s="4" t="s">
         <v>1530</v>
       </c>
-      <c r="T204" s="4"/>
-      <c r="U204" s="4"/>
-      <c r="V204" s="4"/>
-      <c r="W204" s="5"/>
-      <c r="X204" s="8"/>
+      <c r="T204" s="4">
+        <v>685</v>
+      </c>
+      <c r="U204" s="4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="V204" s="4" t="s">
+        <v>1558</v>
+      </c>
+      <c r="W204" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X204" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="205" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A205" s="4"/>
+      <c r="A205" s="4">
+        <f t="shared" si="4"/>
+        <v>204</v>
+      </c>
       <c r="B205" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D205" s="4"/>
-      <c r="E205" s="4"/>
+      <c r="D205" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F205" s="4" t="s">
         <v>28</v>
       </c>
@@ -20354,9 +20511,15 @@
       <c r="J205" s="4" t="s">
         <v>1543</v>
       </c>
-      <c r="K205" s="4"/>
-      <c r="L205" s="4"/>
-      <c r="M205" s="4"/>
+      <c r="K205" s="4">
+        <v>10193146</v>
+      </c>
+      <c r="L205" s="4">
+        <v>70856256</v>
+      </c>
+      <c r="M205" s="4">
+        <v>6945803</v>
+      </c>
       <c r="N205" s="4" t="s">
         <v>762</v>
       </c>
@@ -20366,27 +20529,48 @@
       <c r="P205" s="4" t="s">
         <v>1519</v>
       </c>
-      <c r="Q205" s="4"/>
-      <c r="R205" s="4"/>
+      <c r="Q205" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R205" s="4">
+        <v>82038762</v>
+      </c>
       <c r="S205" s="4" t="s">
         <v>1531</v>
       </c>
-      <c r="T205" s="4"/>
-      <c r="U205" s="4"/>
-      <c r="V205" s="4"/>
-      <c r="W205" s="5"/>
-      <c r="X205" s="8"/>
+      <c r="T205" s="4">
+        <v>684</v>
+      </c>
+      <c r="U205" s="4" t="s">
+        <v>1574</v>
+      </c>
+      <c r="V205" s="4" t="s">
+        <v>1559</v>
+      </c>
+      <c r="W205" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X205" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="206" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="4"/>
+      <c r="A206" s="4">
+        <f t="shared" si="4"/>
+        <v>205</v>
+      </c>
       <c r="B206" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D206" s="4"/>
-      <c r="E206" s="4"/>
+      <c r="D206" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F206" s="4" t="s">
         <v>28</v>
       </c>
@@ -20402,9 +20586,15 @@
       <c r="J206" s="4" t="s">
         <v>1544</v>
       </c>
-      <c r="K206" s="4"/>
-      <c r="L206" s="4"/>
-      <c r="M206" s="4"/>
+      <c r="K206" s="4">
+        <v>10194911</v>
+      </c>
+      <c r="L206" s="4">
+        <v>70856217</v>
+      </c>
+      <c r="M206" s="4">
+        <v>8449389</v>
+      </c>
       <c r="N206" s="4" t="s">
         <v>762</v>
       </c>
@@ -20414,27 +20604,48 @@
       <c r="P206" s="4" t="s">
         <v>1520</v>
       </c>
-      <c r="Q206" s="4"/>
-      <c r="R206" s="4"/>
+      <c r="Q206" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R206" s="4">
+        <v>82038767</v>
+      </c>
       <c r="S206" s="4" t="s">
         <v>1532</v>
       </c>
-      <c r="T206" s="4"/>
-      <c r="U206" s="4"/>
-      <c r="V206" s="4"/>
-      <c r="W206" s="5"/>
-      <c r="X206" s="8"/>
+      <c r="T206" s="4">
+        <v>676</v>
+      </c>
+      <c r="U206" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="V206" s="4" t="s">
+        <v>1560</v>
+      </c>
+      <c r="W206" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X206" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="207" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A207" s="4"/>
+      <c r="A207" s="4">
+        <f t="shared" si="4"/>
+        <v>206</v>
+      </c>
       <c r="B207" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D207" s="4"/>
-      <c r="E207" s="4"/>
+      <c r="D207" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E207" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F207" s="4" t="s">
         <v>28</v>
       </c>
@@ -20450,9 +20661,15 @@
       <c r="J207" s="4" t="s">
         <v>1545</v>
       </c>
-      <c r="K207" s="4"/>
-      <c r="L207" s="4"/>
-      <c r="M207" s="4"/>
+      <c r="K207" s="4">
+        <v>10193099</v>
+      </c>
+      <c r="L207" s="4">
+        <v>70856216</v>
+      </c>
+      <c r="M207" s="4">
+        <v>1165503</v>
+      </c>
       <c r="N207" s="4" t="s">
         <v>762</v>
       </c>
@@ -20462,27 +20679,48 @@
       <c r="P207" s="4" t="s">
         <v>1521</v>
       </c>
-      <c r="Q207" s="4"/>
-      <c r="R207" s="4"/>
+      <c r="Q207" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R207" s="4">
+        <v>82038768</v>
+      </c>
       <c r="S207" s="4" t="s">
         <v>1533</v>
       </c>
-      <c r="T207" s="4"/>
-      <c r="U207" s="4"/>
-      <c r="V207" s="4"/>
-      <c r="W207" s="5"/>
-      <c r="X207" s="8"/>
+      <c r="T207" s="4">
+        <v>677</v>
+      </c>
+      <c r="U207" s="4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="V207" s="4" t="s">
+        <v>1561</v>
+      </c>
+      <c r="W207" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X207" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="208" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A208" s="4"/>
+      <c r="A208" s="4">
+        <f t="shared" si="4"/>
+        <v>207</v>
+      </c>
       <c r="B208" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D208" s="4"/>
-      <c r="E208" s="4"/>
+      <c r="D208" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E208" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F208" s="4" t="s">
         <v>28</v>
       </c>
@@ -20498,9 +20736,15 @@
       <c r="J208" s="4" t="s">
         <v>1546</v>
       </c>
-      <c r="K208" s="4"/>
-      <c r="L208" s="4"/>
-      <c r="M208" s="4"/>
+      <c r="K208" s="4">
+        <v>10207076</v>
+      </c>
+      <c r="L208" s="4">
+        <v>70856259</v>
+      </c>
+      <c r="M208" s="4">
+        <v>6884323</v>
+      </c>
       <c r="N208" s="4" t="s">
         <v>762</v>
       </c>
@@ -20510,27 +20754,48 @@
       <c r="P208" s="4" t="s">
         <v>1522</v>
       </c>
-      <c r="Q208" s="4"/>
-      <c r="R208" s="4"/>
+      <c r="Q208" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R208" s="4">
+        <v>82038761</v>
+      </c>
       <c r="S208" s="4" t="s">
         <v>1534</v>
       </c>
-      <c r="T208" s="4"/>
-      <c r="U208" s="4"/>
-      <c r="V208" s="4"/>
-      <c r="W208" s="5"/>
-      <c r="X208" s="8"/>
+      <c r="T208" s="4">
+        <v>683</v>
+      </c>
+      <c r="U208" s="4" t="s">
+        <v>1577</v>
+      </c>
+      <c r="V208" s="4" t="s">
+        <v>1562</v>
+      </c>
+      <c r="W208" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X208" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="209" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="4"/>
+      <c r="A209" s="4">
+        <f t="shared" si="4"/>
+        <v>208</v>
+      </c>
       <c r="B209" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D209" s="4"/>
-      <c r="E209" s="4"/>
+      <c r="D209" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E209" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F209" s="4" t="s">
         <v>28</v>
       </c>
@@ -20546,9 +20811,15 @@
       <c r="J209" s="4" t="s">
         <v>1547</v>
       </c>
-      <c r="K209" s="4"/>
-      <c r="L209" s="4"/>
-      <c r="M209" s="4"/>
+      <c r="K209" s="4">
+        <v>10230622</v>
+      </c>
+      <c r="L209" s="4">
+        <v>70856220</v>
+      </c>
+      <c r="M209" s="4">
+        <v>8465338</v>
+      </c>
       <c r="N209" s="4" t="s">
         <v>762</v>
       </c>
@@ -20558,27 +20829,48 @@
       <c r="P209" s="4" t="s">
         <v>1523</v>
       </c>
-      <c r="Q209" s="4"/>
-      <c r="R209" s="4"/>
+      <c r="Q209" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R209" s="4">
+        <v>82038769</v>
+      </c>
       <c r="S209" s="4" t="s">
         <v>1535</v>
       </c>
-      <c r="T209" s="4"/>
-      <c r="U209" s="4"/>
-      <c r="V209" s="4"/>
-      <c r="W209" s="5"/>
-      <c r="X209" s="8"/>
+      <c r="T209" s="4">
+        <v>678</v>
+      </c>
+      <c r="U209" s="4" t="s">
+        <v>1578</v>
+      </c>
+      <c r="V209" s="4" t="s">
+        <v>1563</v>
+      </c>
+      <c r="W209" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X209" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="210" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="4"/>
+      <c r="A210" s="4">
+        <f t="shared" si="4"/>
+        <v>209</v>
+      </c>
       <c r="B210" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D210" s="4"/>
-      <c r="E210" s="4"/>
+      <c r="D210" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E210" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F210" s="4" t="s">
         <v>28</v>
       </c>
@@ -20594,9 +20886,15 @@
       <c r="J210" s="4" t="s">
         <v>1548</v>
       </c>
-      <c r="K210" s="4"/>
-      <c r="L210" s="4"/>
-      <c r="M210" s="4"/>
+      <c r="K210" s="4">
+        <v>10228329</v>
+      </c>
+      <c r="L210" s="4">
+        <v>70856219</v>
+      </c>
+      <c r="M210" s="4">
+        <v>3295890</v>
+      </c>
       <c r="N210" s="4" t="s">
         <v>762</v>
       </c>
@@ -20606,27 +20904,48 @@
       <c r="P210" s="4" t="s">
         <v>1524</v>
       </c>
-      <c r="Q210" s="4"/>
-      <c r="R210" s="4"/>
+      <c r="Q210" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R210" s="4">
+        <v>82038770</v>
+      </c>
       <c r="S210" s="4" t="s">
         <v>1536</v>
       </c>
-      <c r="T210" s="4"/>
-      <c r="U210" s="4"/>
-      <c r="V210" s="4"/>
-      <c r="W210" s="5"/>
-      <c r="X210" s="8"/>
+      <c r="T210" s="4">
+        <v>679</v>
+      </c>
+      <c r="U210" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="V210" s="4" t="s">
+        <v>1564</v>
+      </c>
+      <c r="W210" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X210" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="211" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A211" s="4"/>
+      <c r="A211" s="4">
+        <f t="shared" si="4"/>
+        <v>210</v>
+      </c>
       <c r="B211" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D211" s="4"/>
-      <c r="E211" s="4"/>
+      <c r="D211" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E211" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F211" s="4" t="s">
         <v>28</v>
       </c>
@@ -20642,9 +20961,15 @@
       <c r="J211" s="4" t="s">
         <v>1549</v>
       </c>
-      <c r="K211" s="4"/>
-      <c r="L211" s="4"/>
-      <c r="M211" s="4"/>
+      <c r="K211" s="4">
+        <v>10193044</v>
+      </c>
+      <c r="L211" s="4">
+        <v>70856257</v>
+      </c>
+      <c r="M211" s="4">
+        <v>7773749</v>
+      </c>
       <c r="N211" s="4" t="s">
         <v>762</v>
       </c>
@@ -20654,27 +20979,48 @@
       <c r="P211" s="4" t="s">
         <v>1525</v>
       </c>
-      <c r="Q211" s="4"/>
-      <c r="R211" s="4"/>
+      <c r="Q211" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R211" s="4">
+        <v>82038759</v>
+      </c>
       <c r="S211" s="4" t="s">
         <v>1537</v>
       </c>
-      <c r="T211" s="4"/>
-      <c r="U211" s="4"/>
-      <c r="V211" s="4"/>
-      <c r="W211" s="5"/>
-      <c r="X211" s="8"/>
+      <c r="T211" s="4">
+        <v>681</v>
+      </c>
+      <c r="U211" s="4" t="s">
+        <v>1580</v>
+      </c>
+      <c r="V211" s="4" t="s">
+        <v>1565</v>
+      </c>
+      <c r="W211" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X211" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="212" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="4"/>
+      <c r="A212" s="4">
+        <f t="shared" si="4"/>
+        <v>211</v>
+      </c>
       <c r="B212" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D212" s="4"/>
-      <c r="E212" s="4"/>
+      <c r="D212" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E212" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F212" s="4" t="s">
         <v>28</v>
       </c>
@@ -20690,9 +21036,15 @@
       <c r="J212" s="4" t="s">
         <v>1550</v>
       </c>
-      <c r="K212" s="4"/>
-      <c r="L212" s="4"/>
-      <c r="M212" s="4"/>
+      <c r="K212" s="4">
+        <v>10197796</v>
+      </c>
+      <c r="L212" s="4">
+        <v>70856258</v>
+      </c>
+      <c r="M212" s="4">
+        <v>8624718</v>
+      </c>
       <c r="N212" s="4" t="s">
         <v>762</v>
       </c>
@@ -20702,27 +21054,48 @@
       <c r="P212" s="4" t="s">
         <v>1526</v>
       </c>
-      <c r="Q212" s="4"/>
-      <c r="R212" s="4"/>
+      <c r="Q212" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R212" s="4">
+        <v>82038760</v>
+      </c>
       <c r="S212" s="4" t="s">
         <v>1538</v>
       </c>
-      <c r="T212" s="4"/>
-      <c r="U212" s="4"/>
-      <c r="V212" s="4"/>
-      <c r="W212" s="5"/>
-      <c r="X212" s="8"/>
+      <c r="T212" s="4">
+        <v>682</v>
+      </c>
+      <c r="U212" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="V212" s="4" t="s">
+        <v>1566</v>
+      </c>
+      <c r="W212" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X212" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="213" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A213" s="4"/>
+      <c r="A213" s="4">
+        <f t="shared" si="4"/>
+        <v>212</v>
+      </c>
       <c r="B213" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D213" s="4"/>
-      <c r="E213" s="4"/>
+      <c r="D213" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E213" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F213" s="4" t="s">
         <v>28</v>
       </c>
@@ -20738,9 +21111,15 @@
       <c r="J213" s="4" t="s">
         <v>1551</v>
       </c>
-      <c r="K213" s="4"/>
-      <c r="L213" s="4"/>
-      <c r="M213" s="4"/>
+      <c r="K213" s="4">
+        <v>10217149</v>
+      </c>
+      <c r="L213" s="4">
+        <v>70856218</v>
+      </c>
+      <c r="M213" s="4">
+        <v>5719941</v>
+      </c>
       <c r="N213" s="4" t="s">
         <v>762</v>
       </c>
@@ -20750,27 +21129,48 @@
       <c r="P213" s="4" t="s">
         <v>1527</v>
       </c>
-      <c r="Q213" s="4"/>
-      <c r="R213" s="4"/>
+      <c r="Q213" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R213" s="4">
+        <v>82038771</v>
+      </c>
       <c r="S213" s="4" t="s">
         <v>1539</v>
       </c>
-      <c r="T213" s="4"/>
-      <c r="U213" s="4"/>
-      <c r="V213" s="4"/>
-      <c r="W213" s="5"/>
-      <c r="X213" s="8"/>
+      <c r="T213" s="4">
+        <v>680</v>
+      </c>
+      <c r="U213" s="4" t="s">
+        <v>1582</v>
+      </c>
+      <c r="V213" s="4" t="s">
+        <v>1567</v>
+      </c>
+      <c r="W213" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X213" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="214" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="4"/>
+      <c r="A214" s="4">
+        <f t="shared" si="4"/>
+        <v>213</v>
+      </c>
       <c r="B214" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D214" s="4"/>
-      <c r="E214" s="4"/>
+      <c r="D214" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E214" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F214" s="4" t="s">
         <v>28</v>
       </c>
@@ -20786,9 +21186,15 @@
       <c r="J214" s="4" t="s">
         <v>1552</v>
       </c>
-      <c r="K214" s="4"/>
-      <c r="L214" s="4"/>
-      <c r="M214" s="4"/>
+      <c r="K214" s="4">
+        <v>10193115</v>
+      </c>
+      <c r="L214" s="4">
+        <v>70856262</v>
+      </c>
+      <c r="M214" s="4">
+        <v>414724</v>
+      </c>
       <c r="N214" s="4" t="s">
         <v>762</v>
       </c>
@@ -20798,27 +21204,48 @@
       <c r="P214" s="4" t="s">
         <v>1528</v>
       </c>
-      <c r="Q214" s="4"/>
-      <c r="R214" s="4"/>
+      <c r="Q214" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R214" s="4">
+        <v>82038766</v>
+      </c>
       <c r="S214" s="4" t="s">
         <v>1540</v>
       </c>
-      <c r="T214" s="4"/>
-      <c r="U214" s="4"/>
-      <c r="V214" s="4"/>
-      <c r="W214" s="5"/>
-      <c r="X214" s="8"/>
+      <c r="T214" s="4">
+        <v>687</v>
+      </c>
+      <c r="U214" s="4" t="s">
+        <v>1583</v>
+      </c>
+      <c r="V214" s="4" t="s">
+        <v>1568</v>
+      </c>
+      <c r="W214" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X214" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="215" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A215" s="4"/>
+      <c r="A215" s="4">
+        <f t="shared" si="4"/>
+        <v>214</v>
+      </c>
       <c r="B215" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="D215" s="4"/>
-      <c r="E215" s="4"/>
+      <c r="D215" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E215" s="4" t="s">
+        <v>1015</v>
+      </c>
       <c r="F215" s="4" t="s">
         <v>28</v>
       </c>
@@ -20834,9 +21261,15 @@
       <c r="J215" s="4" t="s">
         <v>1553</v>
       </c>
-      <c r="K215" s="4"/>
-      <c r="L215" s="4"/>
-      <c r="M215" s="4"/>
+      <c r="K215" s="4">
+        <v>10220443</v>
+      </c>
+      <c r="L215" s="4">
+        <v>70856260</v>
+      </c>
+      <c r="M215" s="4">
+        <v>451353</v>
+      </c>
       <c r="N215" s="4" t="s">
         <v>762</v>
       </c>
@@ -20846,21 +21279,35 @@
       <c r="P215" s="4" t="s">
         <v>1529</v>
       </c>
-      <c r="Q215" s="4"/>
-      <c r="R215" s="4"/>
+      <c r="Q215" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R215" s="4">
+        <v>82038765</v>
+      </c>
       <c r="S215" s="4" t="s">
         <v>1541</v>
       </c>
-      <c r="T215" s="4"/>
-      <c r="U215" s="4"/>
-      <c r="V215" s="4"/>
-      <c r="W215" s="5"/>
-      <c r="X215" s="8"/>
+      <c r="T215" s="4">
+        <v>686</v>
+      </c>
+      <c r="U215" s="4" t="s">
+        <v>1584</v>
+      </c>
+      <c r="V215" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="W215" s="5">
+        <v>45896</v>
+      </c>
+      <c r="X215" s="8" t="s">
+        <v>1570</v>
+      </c>
     </row>
     <row r="216" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
-        <f>+A203+1</f>
-        <v>203</v>
+        <f t="shared" si="4"/>
+        <v>215</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>28</v>
@@ -20935,7 +21382,7 @@
     <row r="217" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <f t="shared" si="4"/>
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>28</v>
@@ -21010,7 +21457,7 @@
     <row r="218" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <f t="shared" si="4"/>
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="B218" s="4" t="s">
         <v>28</v>
@@ -21085,7 +21532,7 @@
     <row r="219" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <f t="shared" si="4"/>
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B219" s="4" t="s">
         <v>28</v>
@@ -21160,7 +21607,7 @@
     <row r="220" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <f t="shared" si="4"/>
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>28</v>
@@ -21235,7 +21682,7 @@
     <row r="221" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <f t="shared" si="4"/>
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="B221" s="4" t="s">
         <v>28</v>
@@ -21310,7 +21757,7 @@
     <row r="222" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <f t="shared" si="4"/>
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>28</v>
@@ -21385,7 +21832,7 @@
     <row r="223" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <f t="shared" si="4"/>
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B223" s="4" t="s">
         <v>28</v>
@@ -21460,7 +21907,7 @@
     <row r="224" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <f t="shared" si="4"/>
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>28</v>
@@ -21535,7 +21982,7 @@
     <row r="225" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <f t="shared" si="4"/>
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B225" s="4" t="s">
         <v>28</v>
@@ -21610,7 +22057,7 @@
     <row r="226" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <f t="shared" si="4"/>
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="B226" s="4" t="s">
         <v>28</v>
@@ -21685,7 +22132,7 @@
     <row r="227" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <f t="shared" si="4"/>
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B227" s="4" t="s">
         <v>28</v>
@@ -21760,7 +22207,7 @@
     <row r="228" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <f t="shared" si="4"/>
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="B228" s="4" t="s">
         <v>28</v>
@@ -21835,7 +22282,7 @@
     <row r="229" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <f t="shared" si="4"/>
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="B229" s="4" t="s">
         <v>28</v>
@@ -21910,7 +22357,7 @@
     <row r="230" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <f t="shared" si="4"/>
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="B230" s="4" t="s">
         <v>28</v>
@@ -21985,7 +22432,7 @@
     <row r="231" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <f t="shared" si="4"/>
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B231" s="4" t="s">
         <v>28</v>
@@ -22060,7 +22507,7 @@
     <row r="232" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <f t="shared" si="4"/>
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="B232" s="4" t="s">
         <v>28</v>
@@ -22135,7 +22582,7 @@
     <row r="233" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <f t="shared" si="4"/>
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B233" s="4" t="s">
         <v>28</v>
@@ -22210,7 +22657,7 @@
     <row r="234" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <f t="shared" si="4"/>
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B234" s="4" t="s">
         <v>19</v>
@@ -22283,7 +22730,7 @@
     <row r="235" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <f t="shared" si="4"/>
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B235" s="4" t="s">
         <v>19</v>
@@ -22356,7 +22803,7 @@
     <row r="236" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <f t="shared" si="4"/>
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B236" s="4" t="s">
         <v>19</v>
@@ -22429,7 +22876,7 @@
     <row r="237" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <f t="shared" si="4"/>
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B237" s="4" t="s">
         <v>19</v>
@@ -22502,7 +22949,7 @@
     <row r="238" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <f t="shared" si="4"/>
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="B238" s="4" t="s">
         <v>19</v>
@@ -22575,7 +23022,7 @@
     <row r="239" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <f t="shared" si="4"/>
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B239" s="4" t="s">
         <v>19</v>
@@ -22648,7 +23095,7 @@
     <row r="240" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <f t="shared" si="4"/>
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="B240" s="4" t="s">
         <v>19</v>
@@ -22721,7 +23168,7 @@
     <row r="241" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <f t="shared" si="4"/>
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="B241" s="4" t="s">
         <v>19</v>
@@ -22794,7 +23241,7 @@
     <row r="242" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <f t="shared" si="4"/>
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B242" s="4" t="s">
         <v>19</v>
@@ -22867,7 +23314,7 @@
     <row r="243" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <f t="shared" si="4"/>
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B243" s="4" t="s">
         <v>19</v>
@@ -22940,7 +23387,7 @@
     <row r="244" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <f t="shared" si="4"/>
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="B244" s="4" t="s">
         <v>19</v>
@@ -23013,7 +23460,7 @@
     <row r="245" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <f t="shared" si="4"/>
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B245" s="4" t="s">
         <v>19</v>
@@ -23088,7 +23535,7 @@
     <row r="246" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <f t="shared" si="4"/>
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="B246" s="4" t="s">
         <v>19</v>
@@ -23163,7 +23610,7 @@
     <row r="247" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <f t="shared" si="4"/>
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B247" s="4" t="s">
         <v>19</v>
@@ -23238,7 +23685,7 @@
     <row r="248" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <f t="shared" si="4"/>
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="B248" s="4" t="s">
         <v>19</v>
@@ -23313,7 +23760,7 @@
     <row r="249" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <f t="shared" si="4"/>
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B249" s="4" t="s">
         <v>19</v>
@@ -23388,7 +23835,7 @@
     <row r="250" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <f t="shared" si="4"/>
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="B250" s="4" t="s">
         <v>19</v>
@@ -23463,7 +23910,7 @@
     <row r="251" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <f t="shared" si="4"/>
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B251" s="4" t="s">
         <v>19</v>
@@ -23538,7 +23985,7 @@
     <row r="252" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <f t="shared" si="4"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="B252" s="4" t="s">
         <v>19</v>
@@ -23613,7 +24060,7 @@
     <row r="253" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B253" s="4" t="s">
         <v>19</v>
@@ -23686,7 +24133,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X253" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="U2:U253">
     <cfRule type="duplicateValues" dxfId="10" priority="102"/>
   </conditionalFormatting>
@@ -23700,7 +24146,7 @@
   <conditionalFormatting sqref="U166:U191">
     <cfRule type="duplicateValues" dxfId="6" priority="93"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U192:U229">
+  <conditionalFormatting sqref="U192:U203 U216:U229">
     <cfRule type="duplicateValues" dxfId="5" priority="94"/>
     <cfRule type="duplicateValues" dxfId="4" priority="95"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Partners to Sub Retailers
</commit_message>
<xml_diff>
--- a/Calling_Trees/Calling Tree - Aug-25.xlsx
+++ b/Calling_Trees/Calling Tree - Aug-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://xclusivetrading-my.sharepoint.com/personal/m_mahee_xclusivetradinginc_com/Documents/Desktop/Python/Calling Tree Dashboard/CallingTree_Dashboard/Calling_Trees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{443089ED-E8E2-44A4-B672-0F8AB15D6A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F5BD554-2DE5-4B46-9E06-F14E64EEA9FE}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{443089ED-E8E2-44A4-B672-0F8AB15D6A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FF0056A-91F4-45EA-81BB-5BA556C70F57}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4574,9 +4574,6 @@
     <t>INCUBATOR TRAINING STORE</t>
   </si>
   <si>
-    <t>PARTNER</t>
-  </si>
-  <si>
     <t>14703 RINALDI ST STE C</t>
   </si>
   <si>
@@ -4794,6 +4791,9 @@
   </si>
   <si>
     <t xml:space="preserve"> +1 (786) 652-9740</t>
+  </si>
+  <si>
+    <t>SUB RETAILER</t>
   </si>
 </sst>
 </file>
@@ -5371,9 +5371,9 @@
   </sheetPr>
   <dimension ref="A1:X253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8493,7 +8493,7 @@
         <v>1011</v>
       </c>
       <c r="Q42" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R42" s="4">
         <v>82038716</v>
@@ -8568,7 +8568,7 @@
         <v>1012</v>
       </c>
       <c r="Q43" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R43" s="4">
         <v>82038718</v>
@@ -8643,7 +8643,7 @@
         <v>1013</v>
       </c>
       <c r="Q44" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R44" s="4">
         <v>82038719</v>
@@ -8718,7 +8718,7 @@
         <v>1014</v>
       </c>
       <c r="Q45" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R45" s="4">
         <v>82038717</v>
@@ -8772,7 +8772,7 @@
         <v>1010</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="K46" s="4">
         <v>10211200</v>
@@ -8790,31 +8790,31 @@
         <v>1005</v>
       </c>
       <c r="P46" s="4" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="Q46" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R46" s="4">
         <v>82038750</v>
       </c>
       <c r="S46" s="4" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="T46" s="4">
         <v>688</v>
       </c>
       <c r="U46" s="4" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="V46" s="4" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="W46" s="5">
         <v>45896</v>
       </c>
       <c r="X46" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8847,7 +8847,7 @@
         <v>1010</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="K47" s="4">
         <v>10231989</v>
@@ -8865,31 +8865,31 @@
         <v>1005</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="Q47" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R47" s="4">
         <v>82038751</v>
       </c>
       <c r="S47" s="4" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="T47" s="4">
         <v>689</v>
       </c>
       <c r="U47" s="4" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="V47" s="4" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="W47" s="5">
         <v>45896</v>
       </c>
       <c r="X47" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -16214,7 +16214,7 @@
         <v>594</v>
       </c>
       <c r="Q147" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R147" s="4">
         <v>82037237</v>
@@ -16289,7 +16289,7 @@
         <v>597</v>
       </c>
       <c r="Q148" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R148" s="4">
         <v>82037236</v>
@@ -16364,7 +16364,7 @@
         <v>600</v>
       </c>
       <c r="Q149" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R149" s="4">
         <v>82037234</v>
@@ -16439,7 +16439,7 @@
         <v>603</v>
       </c>
       <c r="Q150" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R150" s="4">
         <v>82037235</v>
@@ -16514,7 +16514,7 @@
         <v>606</v>
       </c>
       <c r="Q151" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R151" s="4">
         <v>82037232</v>
@@ -16589,7 +16589,7 @@
         <v>609</v>
       </c>
       <c r="Q152" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R152" s="4">
         <v>82037222</v>
@@ -16664,7 +16664,7 @@
         <v>612</v>
       </c>
       <c r="Q153" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R153" s="4">
         <v>82037233</v>
@@ -16739,7 +16739,7 @@
         <v>615</v>
       </c>
       <c r="Q154" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R154" s="4">
         <v>82037224</v>
@@ -16814,7 +16814,7 @@
         <v>618</v>
       </c>
       <c r="Q155" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R155" s="4">
         <v>82037226</v>
@@ -16889,7 +16889,7 @@
         <v>621</v>
       </c>
       <c r="Q156" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R156" s="4">
         <v>82037231</v>
@@ -16964,7 +16964,7 @@
         <v>624</v>
       </c>
       <c r="Q157" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R157" s="4">
         <v>82037223</v>
@@ -17039,7 +17039,7 @@
         <v>627</v>
       </c>
       <c r="Q158" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R158" s="4">
         <v>82037225</v>
@@ -17114,7 +17114,7 @@
         <v>630</v>
       </c>
       <c r="Q159" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R159" s="4">
         <v>82037227</v>
@@ -17189,7 +17189,7 @@
         <v>633</v>
       </c>
       <c r="Q160" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R160" s="4">
         <v>82037229</v>
@@ -17264,7 +17264,7 @@
         <v>636</v>
       </c>
       <c r="Q161" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R161" s="4">
         <v>82037228</v>
@@ -19552,7 +19552,7 @@
         <v>762</v>
       </c>
       <c r="P192" s="4" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="Q192" s="4" t="s">
         <v>1507</v>
@@ -20152,7 +20152,7 @@
         <v>762</v>
       </c>
       <c r="P200" s="4" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="Q200" s="4" t="s">
         <v>1507</v>
@@ -20434,7 +20434,7 @@
         <v>760</v>
       </c>
       <c r="J204" s="4" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="K204" s="4">
         <v>10210174</v>
@@ -20452,7 +20452,7 @@
         <v>762</v>
       </c>
       <c r="P204" s="4" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="Q204" s="4" t="s">
         <v>1507</v>
@@ -20461,22 +20461,22 @@
         <v>82038763</v>
       </c>
       <c r="S204" s="4" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="T204" s="4">
         <v>685</v>
       </c>
       <c r="U204" s="4" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="V204" s="4" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="W204" s="5">
         <v>45896</v>
       </c>
       <c r="X204" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="205" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20509,7 +20509,7 @@
         <v>760</v>
       </c>
       <c r="J205" s="4" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="K205" s="4">
         <v>10193146</v>
@@ -20527,7 +20527,7 @@
         <v>762</v>
       </c>
       <c r="P205" s="4" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="Q205" s="4" t="s">
         <v>1507</v>
@@ -20536,22 +20536,22 @@
         <v>82038762</v>
       </c>
       <c r="S205" s="4" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="T205" s="4">
         <v>684</v>
       </c>
       <c r="U205" s="4" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="V205" s="4" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="W205" s="5">
         <v>45896</v>
       </c>
       <c r="X205" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="206" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20584,7 +20584,7 @@
         <v>760</v>
       </c>
       <c r="J206" s="4" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="K206" s="4">
         <v>10194911</v>
@@ -20602,7 +20602,7 @@
         <v>762</v>
       </c>
       <c r="P206" s="4" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="Q206" s="4" t="s">
         <v>1507</v>
@@ -20611,22 +20611,22 @@
         <v>82038767</v>
       </c>
       <c r="S206" s="4" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="T206" s="4">
         <v>676</v>
       </c>
       <c r="U206" s="4" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="V206" s="4" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="W206" s="5">
         <v>45896</v>
       </c>
       <c r="X206" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="207" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20659,7 +20659,7 @@
         <v>760</v>
       </c>
       <c r="J207" s="4" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="K207" s="4">
         <v>10193099</v>
@@ -20677,7 +20677,7 @@
         <v>762</v>
       </c>
       <c r="P207" s="4" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="Q207" s="4" t="s">
         <v>1507</v>
@@ -20686,22 +20686,22 @@
         <v>82038768</v>
       </c>
       <c r="S207" s="4" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="T207" s="4">
         <v>677</v>
       </c>
       <c r="U207" s="4" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="V207" s="4" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="W207" s="5">
         <v>45896</v>
       </c>
       <c r="X207" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="208" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20734,7 +20734,7 @@
         <v>760</v>
       </c>
       <c r="J208" s="4" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="K208" s="4">
         <v>10207076</v>
@@ -20752,7 +20752,7 @@
         <v>762</v>
       </c>
       <c r="P208" s="4" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="Q208" s="4" t="s">
         <v>1507</v>
@@ -20761,22 +20761,22 @@
         <v>82038761</v>
       </c>
       <c r="S208" s="4" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="T208" s="4">
         <v>683</v>
       </c>
       <c r="U208" s="4" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="V208" s="4" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="W208" s="5">
         <v>45896</v>
       </c>
       <c r="X208" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="209" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20809,7 +20809,7 @@
         <v>760</v>
       </c>
       <c r="J209" s="4" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="K209" s="4">
         <v>10230622</v>
@@ -20827,7 +20827,7 @@
         <v>762</v>
       </c>
       <c r="P209" s="4" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="Q209" s="4" t="s">
         <v>1507</v>
@@ -20836,22 +20836,22 @@
         <v>82038769</v>
       </c>
       <c r="S209" s="4" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="T209" s="4">
         <v>678</v>
       </c>
       <c r="U209" s="4" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="V209" s="4" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="W209" s="5">
         <v>45896</v>
       </c>
       <c r="X209" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="210" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20884,7 +20884,7 @@
         <v>760</v>
       </c>
       <c r="J210" s="4" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="K210" s="4">
         <v>10228329</v>
@@ -20902,7 +20902,7 @@
         <v>762</v>
       </c>
       <c r="P210" s="4" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="Q210" s="4" t="s">
         <v>1507</v>
@@ -20911,22 +20911,22 @@
         <v>82038770</v>
       </c>
       <c r="S210" s="4" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="T210" s="4">
         <v>679</v>
       </c>
       <c r="U210" s="4" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="V210" s="4" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="W210" s="5">
         <v>45896</v>
       </c>
       <c r="X210" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="211" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -20959,7 +20959,7 @@
         <v>760</v>
       </c>
       <c r="J211" s="4" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="K211" s="4">
         <v>10193044</v>
@@ -20977,7 +20977,7 @@
         <v>762</v>
       </c>
       <c r="P211" s="4" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="Q211" s="4" t="s">
         <v>1507</v>
@@ -20986,22 +20986,22 @@
         <v>82038759</v>
       </c>
       <c r="S211" s="4" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="T211" s="4">
         <v>681</v>
       </c>
       <c r="U211" s="4" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="V211" s="4" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="W211" s="5">
         <v>45896</v>
       </c>
       <c r="X211" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="212" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -21034,7 +21034,7 @@
         <v>760</v>
       </c>
       <c r="J212" s="4" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="K212" s="4">
         <v>10197796</v>
@@ -21052,7 +21052,7 @@
         <v>762</v>
       </c>
       <c r="P212" s="4" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="Q212" s="4" t="s">
         <v>1507</v>
@@ -21061,22 +21061,22 @@
         <v>82038760</v>
       </c>
       <c r="S212" s="4" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="T212" s="4">
         <v>682</v>
       </c>
       <c r="U212" s="4" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="V212" s="4" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="W212" s="5">
         <v>45896</v>
       </c>
       <c r="X212" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="213" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -21109,7 +21109,7 @@
         <v>760</v>
       </c>
       <c r="J213" s="4" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="K213" s="4">
         <v>10217149</v>
@@ -21127,7 +21127,7 @@
         <v>762</v>
       </c>
       <c r="P213" s="4" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="Q213" s="4" t="s">
         <v>1507</v>
@@ -21136,22 +21136,22 @@
         <v>82038771</v>
       </c>
       <c r="S213" s="4" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="T213" s="4">
         <v>680</v>
       </c>
       <c r="U213" s="4" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="V213" s="4" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="W213" s="5">
         <v>45896</v>
       </c>
       <c r="X213" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="214" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -21184,7 +21184,7 @@
         <v>760</v>
       </c>
       <c r="J214" s="4" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="K214" s="4">
         <v>10193115</v>
@@ -21202,7 +21202,7 @@
         <v>762</v>
       </c>
       <c r="P214" s="4" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="Q214" s="4" t="s">
         <v>1507</v>
@@ -21211,22 +21211,22 @@
         <v>82038766</v>
       </c>
       <c r="S214" s="4" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="T214" s="4">
         <v>687</v>
       </c>
       <c r="U214" s="4" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="V214" s="4" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="W214" s="5">
         <v>45896</v>
       </c>
       <c r="X214" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="215" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -21259,7 +21259,7 @@
         <v>760</v>
       </c>
       <c r="J215" s="4" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="K215" s="4">
         <v>10220443</v>
@@ -21277,7 +21277,7 @@
         <v>762</v>
       </c>
       <c r="P215" s="4" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="Q215" s="4" t="s">
         <v>1507</v>
@@ -21286,22 +21286,22 @@
         <v>82038765</v>
       </c>
       <c r="S215" s="4" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="T215" s="4">
         <v>686</v>
       </c>
       <c r="U215" s="4" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="V215" s="4" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="W215" s="5">
         <v>45896</v>
       </c>
       <c r="X215" s="8" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="216" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -21355,7 +21355,7 @@
         <v>815</v>
       </c>
       <c r="Q216" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R216" s="4">
         <v>82037536</v>
@@ -21430,7 +21430,7 @@
         <v>818</v>
       </c>
       <c r="Q217" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R217" s="4">
         <v>82037540</v>
@@ -21505,7 +21505,7 @@
         <v>821</v>
       </c>
       <c r="Q218" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R218" s="4">
         <v>82037561</v>
@@ -21580,7 +21580,7 @@
         <v>824</v>
       </c>
       <c r="Q219" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R219" s="4">
         <v>82037564</v>
@@ -21655,7 +21655,7 @@
         <v>827</v>
       </c>
       <c r="Q220" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R220" s="4">
         <v>82037569</v>
@@ -21730,7 +21730,7 @@
         <v>830</v>
       </c>
       <c r="Q221" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R221" s="4">
         <v>82037573</v>
@@ -21805,7 +21805,7 @@
         <v>835</v>
       </c>
       <c r="Q222" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R222" s="4">
         <v>82037544</v>
@@ -21880,7 +21880,7 @@
         <v>838</v>
       </c>
       <c r="Q223" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R223" s="4">
         <v>82037548</v>
@@ -21955,7 +21955,7 @@
         <v>841</v>
       </c>
       <c r="Q224" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R224" s="4">
         <v>82037552</v>
@@ -22030,7 +22030,7 @@
         <v>844</v>
       </c>
       <c r="Q225" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R225" s="4">
         <v>82037523</v>
@@ -22105,7 +22105,7 @@
         <v>847</v>
       </c>
       <c r="Q226" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R226" s="4">
         <v>82037529</v>
@@ -22180,7 +22180,7 @@
         <v>850</v>
       </c>
       <c r="Q227" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R227" s="4">
         <v>82037531</v>
@@ -22255,7 +22255,7 @@
         <v>853</v>
       </c>
       <c r="Q228" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R228" s="4">
         <v>82037533</v>
@@ -22330,7 +22330,7 @@
         <v>856</v>
       </c>
       <c r="Q229" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R229" s="4">
         <v>82037556</v>
@@ -22405,7 +22405,7 @@
         <v>859</v>
       </c>
       <c r="Q230" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R230" s="4">
         <v>82037524</v>
@@ -22480,7 +22480,7 @@
         <v>862</v>
       </c>
       <c r="Q231" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R231" s="4">
         <v>82037525</v>
@@ -22555,7 +22555,7 @@
         <v>865</v>
       </c>
       <c r="Q232" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R232" s="4">
         <v>82037526</v>
@@ -22630,7 +22630,7 @@
         <v>868</v>
       </c>
       <c r="Q233" s="4" t="s">
-        <v>1511</v>
+        <v>1584</v>
       </c>
       <c r="R233" s="4">
         <v>82037528</v>
@@ -24133,6 +24133,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:X253" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="U2:U253">
     <cfRule type="duplicateValues" dxfId="10" priority="102"/>
   </conditionalFormatting>

</xml_diff>